<commit_message>
Checkpoint quase a entrega.
</commit_message>
<xml_diff>
--- a/Trabalho Jean Rangel/arquivos/cronograma.xlsx
+++ b/Trabalho Jean Rangel/arquivos/cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Jun</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Ok</t>
   </si>
   <si>
-    <t>Não Inic.</t>
-  </si>
-  <si>
     <t>Elaborar o método de pesquisa.</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Produzir artigo científico.</t>
   </si>
   <si>
-    <t>Publicar artigo finalizado.</t>
-  </si>
-  <si>
     <t>Definir objetivos, justificativa e motivação.</t>
   </si>
   <si>
@@ -72,13 +66,16 @@
   </si>
   <si>
     <t>Revisar a literatura e selecionar trabalhos.</t>
+  </si>
+  <si>
+    <t>Submeter para a banca e publicar o artigo finalizado.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +105,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -124,18 +128,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF7D7D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -182,15 +186,12 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -201,10 +202,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,40 +501,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="6" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1"/>
@@ -538,10 +542,10 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1"/>
@@ -549,10 +553,10 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1"/>
@@ -560,10 +564,10 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1"/>
@@ -571,42 +575,40 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>15</v>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>6</v>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>11</v>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>12</v>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>